<commit_message>
update plan and files
</commit_message>
<xml_diff>
--- a/subject__information_science/Max_Heap.xlsx
+++ b/subject__information_science/Max_Heap.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PyuDi\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\cnsh_files\subject__information_science\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6E03D59-BB7F-4410-8DF2-147AF6AD8148}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA7F45F4-0540-4204-BCBB-6C2ED01A20C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -105,44 +105,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>H[1]&lt;H[2]
-9 &gt; 7</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>end</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>H[1]&lt;H[3]
-9 &gt; 3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>H[1]&lt;H[2]
-9 &gt; 6</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>end</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>H[2]&lt;H[5]
-6 &gt; 4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>H[6]=2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>up(6)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>H[3]&lt;H[6]
-3 &gt; 2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -190,11 +165,6 @@
   </si>
   <si>
     <t>up(3)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>H[1]&lt;H[3]
-9 &gt; 5</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -221,11 +191,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>H[4]&lt;H[8]
-6 &gt; 1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>H[4]&lt;H[9]
 6 &lt; 8</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -258,32 +223,67 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>True/False</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>continue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>H[k/2]&lt;H[k]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>up 종료여부</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>작업</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>H[1]&lt;H[2]
-9 &gt; 8</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>True/False</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>continue</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>s</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>H[k/2]&lt;H[k]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>up 종료여부</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>작업</t>
+9 &lt; 8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>H[4]&lt;H[8]
+6 &lt; 1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>H[1]&lt;H[3]
+9 &lt; 5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>H[3]&lt;H[6]
+3 &lt; 2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>H[2]&lt;H[5]
+6 &lt; 4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>H[1]&lt;H[2]
+9 &lt; 7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>H[1]&lt;H[3]
+9 &lt; 3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>H[1]&lt;H[2]
+9 &lt; 6</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -744,10 +744,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:S14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="101" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S7" sqref="S7"/>
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -776,7 +779,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>3</v>
@@ -785,43 +788,43 @@
         <v>4</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="J1" s="13" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="K1" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="P1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>31</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="P1" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q1" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="R1" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="S1" s="5" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
@@ -853,7 +856,7 @@
         <v>15</v>
       </c>
       <c r="J2" s="14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K2" s="12">
         <v>9</v>
@@ -887,7 +890,7 @@
         <v>2</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>22</v>
+        <v>60</v>
       </c>
       <c r="H3" s="8" t="b">
         <v>0</v>
@@ -896,7 +899,7 @@
         <v>17</v>
       </c>
       <c r="J3" s="14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K3" s="11">
         <v>9</v>
@@ -932,7 +935,7 @@
         <v>3</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>21</v>
+        <v>59</v>
       </c>
       <c r="H4" s="8" t="b">
         <v>0</v>
@@ -941,7 +944,7 @@
         <v>17</v>
       </c>
       <c r="J4" s="14" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K4" s="11">
         <v>9</v>
@@ -988,7 +991,7 @@
         <v>16</v>
       </c>
       <c r="J5" s="13" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="K5" s="11">
         <v>9</v>
@@ -1022,7 +1025,7 @@
         <v>4</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>19</v>
+        <v>58</v>
       </c>
       <c r="H6" s="8" t="b">
         <v>0</v>
@@ -1031,7 +1034,7 @@
         <v>17</v>
       </c>
       <c r="J6" s="14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K6" s="11">
         <v>9</v>
@@ -1071,7 +1074,7 @@
         <v>5</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>24</v>
+        <v>57</v>
       </c>
       <c r="H7" s="8" t="b">
         <v>0</v>
@@ -1080,7 +1083,7 @@
         <v>17</v>
       </c>
       <c r="J7" s="14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K7" s="11">
         <v>9</v>
@@ -1110,19 +1113,19 @@
         <v>2</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D8" s="4">
         <v>6</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F8" s="4">
         <v>6</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>27</v>
+        <v>56</v>
       </c>
       <c r="H8" s="8" t="b">
         <v>0</v>
@@ -1131,7 +1134,7 @@
         <v>17</v>
       </c>
       <c r="J8" s="14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K8" s="11">
         <v>9</v>
@@ -1163,28 +1166,28 @@
         <v>5</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D9" s="4">
         <v>7</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="F9" s="4">
         <v>7</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="H9" s="7" t="b">
         <v>1</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="J9" s="13" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="K9" s="11">
         <v>9</v>
@@ -1218,13 +1221,13 @@
         <v>7</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="F10" s="4">
         <v>7</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="H10" s="8" t="b">
         <v>0</v>
@@ -1233,7 +1236,7 @@
         <v>17</v>
       </c>
       <c r="J10" s="14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K10" s="11">
         <v>9</v>
@@ -1267,19 +1270,19 @@
         <v>1</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D11" s="4">
         <v>8</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="F11" s="4">
         <v>8</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="H11" s="8" t="b">
         <v>0</v>
@@ -1288,7 +1291,7 @@
         <v>17</v>
       </c>
       <c r="J11" s="14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K11" s="11">
         <v>9</v>
@@ -1324,28 +1327,28 @@
         <v>8</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D12" s="4">
         <v>9</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="F12" s="4">
         <v>9</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="H12" s="7" t="b">
         <v>1</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="J12" s="13" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="K12" s="11">
         <v>9</v>
@@ -1383,22 +1386,22 @@
         <v>9</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="F13" s="4">
         <v>9</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="H13" s="7" t="b">
         <v>1</v>
       </c>
       <c r="I13" s="9" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="J13" s="13" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="K13" s="11">
         <v>9</v>
@@ -1436,13 +1439,13 @@
         <v>9</v>
       </c>
       <c r="E14" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F14" s="4">
+        <v>9</v>
+      </c>
+      <c r="G14" s="7" t="s">
         <v>53</v>
-      </c>
-      <c r="F14" s="4">
-        <v>9</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>54</v>
       </c>
       <c r="H14" s="8" t="b">
         <v>0</v>
@@ -1451,7 +1454,7 @@
         <v>17</v>
       </c>
       <c r="J14" s="14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K14" s="11">
         <v>9</v>
@@ -1483,7 +1486,10 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="83" fitToWidth="0" orientation="landscape" horizontalDpi="4294967293" verticalDpi="300" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;L&amp;14힙 만드는 과정 분석 (p138)</oddHeader>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>